<commit_message>
update voxmarket, interface clean and scalable
</commit_message>
<xml_diff>
--- a/hrcrm/dict_test.xlsx
+++ b/hrcrm/dict_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,39 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>What is for you Brio Maté ?</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Pour moi, Brio Maté est une très bonne marque de maté parce que c'est sustainable et que le goût est très bon.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Qu'est-ce que vous aimez le plus à propos de Brio Maté ?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Concernant le Brio Maté, ce que j'aime le plus, c'est le nouveau goût avec le limon qui est vraiment très bien.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Quels autres avantages trouvez-vous dans le Brio Maté par rapport à d'autres marques de maté ?</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Les autres avantages, c'est aussi qu'ils livrent super vite. Là, j'ai tout réussi en une journée, donc c'est incroyable.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>